<commit_message>
add imo list rank
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data/templates/ImoList_template.xlsx
+++ b/backend/src/main/resources/data/templates/ImoList_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jana\IdeaProjects\eventplanner\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13F06C7-5DF2-4E9A-9757-90121D46C0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B1D530-88A8-4815-9683-098F282E6A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24630" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>German</t>
   </si>
   <si>
-    <t>11. Nature and No. of identity document  (Passport)</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Arrival</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   <si>
     <t>{{Date_a/d}}</t>
   </si>
+  <si>
+    <t>11. Nature and No. of identity document</t>
+  </si>
 </sst>
 </file>
 
@@ -106,16 +106,9 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -147,12 +140,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -559,94 +546,85 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1069,31 +1047,31 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:G5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1103,7 +1081,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1112,766 +1090,766 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="40" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="15" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="17"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="17"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="17"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="17"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="10"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="17"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="17"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="10"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="17"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="18"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="18"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="18"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="18"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="18"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="18"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="18"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="18"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="18"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="18"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="18"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="18"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="18"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="18"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="18"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="18"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="18"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="18"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="19"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="10"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="17"/>
+      <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="10"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="17"/>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="10"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="17"/>
+      <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="10"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="17"/>
+      <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="2"/>
-      <c r="F50" s="10"/>
+      <c r="F50" s="4"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="17"/>
+      <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="10"/>
+      <c r="F51" s="4"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="17"/>
+      <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="10"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="17"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="10"/>
+      <c r="F53" s="4"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="17"/>
+      <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="10"/>
+      <c r="F54" s="4"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="17"/>
+      <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="10"/>
+      <c r="F55" s="4"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="17"/>
+      <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="31"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="10"/>
+      <c r="F56" s="4"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="17"/>
+      <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="18"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="18"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="18"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="18"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="18"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="18"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="18"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="18"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="18"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="18"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="32"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="18"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="32"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="18"/>
+      <c r="A68" s="16"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="10"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="18"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="18"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="18"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="10"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="32"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="18"/>
+      <c r="A72" s="16"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="10"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="32"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="18"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="32"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="18"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="34"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="29"/>
+      <c r="A75" s="22"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>